<commit_message>
arbeitszeit und ressourcen für doku, also doku
</commit_message>
<xml_diff>
--- a/dokumentation/arbeitszeiten/Arbeitszeiten_grr37213.xlsx
+++ b/dokumentation/arbeitszeiten/Arbeitszeiten_grr37213.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
   <si>
     <t xml:space="preserve">Arbeitszeit je Woche:</t>
   </si>
@@ -86,7 +86,10 @@
     <t xml:space="preserve">Festlegung der Projekte</t>
   </si>
   <si>
-    <t xml:space="preserve">Persönliche Eintragung in Grenn Dia</t>
+    <t xml:space="preserve">Persönliche Eintragung in Grenn Diagramm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erstellung eines Pflichtenheftes via Latex-Template, Latex-Recherche</t>
   </si>
   <si>
     <t xml:space="preserve">Projektbeschreibung / Terminplan</t>
@@ -104,19 +107,19 @@
     <t xml:space="preserve">Iststunden:</t>
   </si>
   <si>
-    <t xml:space="preserve">Programmierkonventionen, Strukturierung</t>
+    <t xml:space="preserve">Programmierkonventionen wurden vereinbart, grobe Strukturierung</t>
   </si>
   <si>
     <t xml:space="preserve">Überlegungen zu Interboardkomminikation dokumentiert , zusätzliche Tex-Recherche</t>
   </si>
   <si>
-    <t xml:space="preserve">Serial Connection erste Versuche in Zusammenarbeit mit bof</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versuch in C++ Komponente umgewandelt, Erweiterung meines Arbeitszeiten-Templates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Überlegungen zur Verteilung von Nachrichten</t>
+    <t xml:space="preserve">Serial Connection erste Versuche in Zusammenarbeit mit Florian Bömmel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versuch zum Seriellen Port in C++ Komponente umgewandelt, Erweiterung meines Arbeitszeiten-Templates durch Teamzeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erste Versuche zur Protokollerstellung [V0.0] und Tests</t>
   </si>
   <si>
     <t xml:space="preserve">Implemetierung weiterer Kontrollstrukturen für Nachrichten</t>
@@ -125,22 +128,25 @@
     <t xml:space="preserve">Packet und Inbox strukturen für Nachrichten implementiert</t>
   </si>
   <si>
-    <t xml:space="preserve">An Organisationsklasse für Serial Header experimentiert, nach hash funktionen recherchiert</t>
+    <t xml:space="preserve">An Organisationsklasse für Serial Header experimentiert, Hash Funktionen recherchiert</t>
   </si>
   <si>
     <t xml:space="preserve">Verbindliche Zielvereinbarung</t>
   </si>
   <si>
-    <t xml:space="preserve">Beginn Refactoring IBC auf Grund von Anforderungsänderungen ()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refactored Protocoll, but made a mistake so it was all for naught</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refactored Protocoll again</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fix errors and implementing more special features , adding TODO tags to what is still missing</t>
+    <t xml:space="preserve">Erster besserer Protokollablauf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IBC-Refactoring wegen Anforderungsänderungen bezüglich Übertragungssicherheit [V0.3]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fortsetzung, Implemetierungsfehler festgestellt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erneutes Reafactoring wegen Implementierungsfehler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fehlerbehebung und Absicherung von Ablaufcode, z.B. Padding</t>
   </si>
   <si>
     <t xml:space="preserve">Simulation der Serial Verbindung für Testvorgänge zu Hause</t>
@@ -158,46 +164,52 @@
     <t xml:space="preserve">Dokumentieren und Kommentieren</t>
   </si>
   <si>
-    <t xml:space="preserve">Sendeprozess thread safe, implementierung von Arduino test cases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vereinfachung der benutzung des Protokolls auf Arduiono Seite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNO code generator und Arduino API</t>
+    <t xml:space="preserve">Sendeprozess thread safe gemacht , implementierung von Arduino test cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vereinfachung der Benutzung des Protokolls auf Arduiono Seite durch IBC-Klasse auf Arduino Seite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arduino-Code Generator in Python und Arduino API verbessert</t>
   </si>
   <si>
     <t xml:space="preserve">Fertigstellung uno code generator</t>
   </si>
   <si>
-    <t xml:space="preserve">Threadsafe storing of answers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Errorhandling on pi side</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fehler einsehen und Nachtschichten einlegen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bereuen Fehler Eingesehen zu haben aber es trotzdem durchziehen alles nochmal neu zu machen, dass es hoffentlich funktioniert.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Segmentation Faults. Inbox Komponente umgeschrieben, folien für ergebnisvorstellung erstellt</t>
+    <t xml:space="preserve">Piseitige Speicherung und Verteilung von Antwortpacketen thread-safe implementiert.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrierungsfehler, Seg-Faults</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versuche, Seg-Fault durch Umschreiben vieler Komponenten zu vermeiden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versuche, Seg-Fault durch Umschreiben vieler Komponenten zu vermeiden und fluchen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weiteres Debugging nach immernoch auftretetenden Segmentation Faults, Erstellung von einigen Folien über IBC, falls für Präsentation benötigt</t>
   </si>
   <si>
     <t xml:space="preserve">Erste Ergebnisvorstellung</t>
   </si>
   <si>
-    <t xml:space="preserve">Umschreiben der Komponenten von std:: nach qt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Presentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">debugging in Protocoll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Issues Flashing uno and debugging protocoll</t>
+    <t xml:space="preserve">Umschreiben der Komponenten von std nach qt um mögliche Fehler zu vermeiden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verbesserter Protokollablauf erdacht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erstellen von Folien für Präsentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oberflächliche Fehlersuche nach Fehlermeldung von Kollegen über falsch übertragenen Sensorwerte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protokollfehler, Fehlersuche nur über Pi-sniffing am Port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Probleme beim Aufsetzen der Entwicklungsumgebung zum Flashen von Arduino,  letztendlich Auslagerung in einen Unittest und weiteres Debugging</t>
   </si>
   <si>
     <t xml:space="preserve">Präsentation bzw. Vorträge</t>
@@ -209,7 +221,13 @@
     <t xml:space="preserve">Dokumentation, Übertrag in Google Doc und Formatierungen</t>
   </si>
   <si>
+    <t xml:space="preserve">Funktionalitätstests für die Vorführung</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vorführung der Ergebnisse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dokumentation, Übertag in Google Doc und Formatierung, Überprüfung des Stundenzettels</t>
   </si>
 </sst>
 </file>
@@ -337,7 +355,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -367,7 +385,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -380,6 +398,10 @@
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -759,8 +781,8 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -768,7 +790,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -797,7 +821,7 @@
       <c r="A4" s="1"/>
       <c r="B4" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -834,7 +858,7 @@
       </c>
       <c r="B8" s="9" t="n">
         <f aca="false">'November 2017'!H34</f>
-        <v>1.80347222222222</v>
+        <v>2.04444444444444</v>
       </c>
       <c r="C8" s="9" t="n">
         <f aca="false">5*B1</f>
@@ -842,7 +866,7 @@
       </c>
       <c r="E8" s="10" t="n">
         <f aca="false">B8/C8</f>
-        <v>0.961851851851851</v>
+        <v>1.09037037037037</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,7 +875,7 @@
       </c>
       <c r="B9" s="9" t="n">
         <f aca="false">'Dezember 2017'!H34</f>
-        <v>2.75416666666667</v>
+        <v>2.8375</v>
       </c>
       <c r="C9" s="9" t="n">
         <f aca="false">4*B1</f>
@@ -859,7 +883,7 @@
       </c>
       <c r="E9" s="10" t="n">
         <f aca="false">B9/C9</f>
-        <v>1.83611111111111</v>
+        <v>1.89166666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -868,7 +892,7 @@
       </c>
       <c r="B10" s="9" t="n">
         <f aca="false">'Januar 2018'!H34</f>
-        <v>1.23680555555556</v>
+        <v>1.77013888888889</v>
       </c>
       <c r="C10" s="9" t="n">
         <f aca="false">5*B1</f>
@@ -876,7 +900,7 @@
       </c>
       <c r="E10" s="10" t="n">
         <f aca="false">B10/C10</f>
-        <v>0.65962962962963</v>
+        <v>0.944074074074074</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -886,12 +910,12 @@
       <c r="E11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="9" t="n">
         <f aca="false">SUM(B7:B10)</f>
-        <v>6.47152777777778</v>
+        <v>7.32916666666666</v>
       </c>
       <c r="C12" s="9" t="n">
         <f aca="false">SUM(C7:C10)</f>
@@ -899,7 +923,7 @@
       </c>
       <c r="E12" s="10" t="n">
         <f aca="false">B12/C12</f>
-        <v>1.01514161220044</v>
+        <v>1.14967320261438</v>
       </c>
     </row>
   </sheetData>
@@ -923,8 +947,8 @@
   </sheetPr>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -940,178 +964,178 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="n">
+      <c r="A2" s="13" t="n">
         <f aca="false">DATE(2017,10,1)</f>
         <v>43009</v>
       </c>
-      <c r="B2" s="13" t="n">
+      <c r="B2" s="14" t="n">
         <f aca="false">A2</f>
         <v>43009</v>
       </c>
-      <c r="C2" s="14" t="n">
+      <c r="C2" s="15" t="n">
         <f aca="false">WEEKNUM(A2,2)</f>
         <v>40</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16" t="n">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17" t="n">
         <f aca="false">(E2-D2-F2+G2)</f>
         <v>0</v>
       </c>
-      <c r="I2" s="17"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="n">
+      <c r="A3" s="13" t="n">
         <f aca="false">A2+1</f>
         <v>43010</v>
       </c>
-      <c r="B3" s="13" t="n">
+      <c r="B3" s="14" t="n">
         <f aca="false">A3</f>
         <v>43010</v>
       </c>
-      <c r="C3" s="14" t="n">
+      <c r="C3" s="15" t="n">
         <f aca="false">WEEKNUM(A3,2)</f>
         <v>41</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="16" t="n">
+      <c r="H3" s="17" t="n">
         <f aca="false">(E3-D3-F3+G3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="n">
+      <c r="A4" s="13" t="n">
         <f aca="false">A3+1</f>
         <v>43011</v>
       </c>
-      <c r="B4" s="13" t="n">
+      <c r="B4" s="14" t="n">
         <f aca="false">A4</f>
         <v>43011</v>
       </c>
-      <c r="C4" s="14" t="n">
+      <c r="C4" s="15" t="n">
         <f aca="false">WEEKNUM(A4,2)</f>
         <v>41</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="16" t="n">
+      <c r="H4" s="17" t="n">
         <f aca="false">(E4-D4-F4+G4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="n">
+      <c r="A5" s="13" t="n">
         <f aca="false">A4+1</f>
         <v>43012</v>
       </c>
-      <c r="B5" s="13" t="n">
+      <c r="B5" s="14" t="n">
         <f aca="false">A5</f>
         <v>43012</v>
       </c>
-      <c r="C5" s="14" t="n">
+      <c r="C5" s="15" t="n">
         <f aca="false">WEEKNUM(A5,2)</f>
         <v>41</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="16" t="n">
+      <c r="H5" s="17" t="n">
         <f aca="false">(E5-D5-F5+G5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="n">
+      <c r="A6" s="13" t="n">
         <f aca="false">A5+1</f>
         <v>43013</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="14" t="n">
+      <c r="C6" s="15" t="n">
         <f aca="false">WEEKNUM(A6,2)</f>
         <v>41</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="16" t="n">
+      <c r="H6" s="17" t="n">
         <f aca="false">(E6-D6-F6+G6)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" s="21" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="n">
+    <row r="7" s="22" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="20" t="n">
         <f aca="false">A6+1</f>
         <v>43014</v>
       </c>
-      <c r="B7" s="20" t="n">
+      <c r="B7" s="21" t="n">
         <f aca="false">A7</f>
         <v>43014</v>
       </c>
-      <c r="C7" s="21" t="n">
+      <c r="C7" s="22" t="n">
         <f aca="false">WEEKNUM(A7,2)</f>
         <v>41</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16" t="n">
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17" t="n">
         <v>0.0625</v>
       </c>
-      <c r="H7" s="16" t="n">
+      <c r="H7" s="17" t="n">
         <f aca="false">(E7-D7-F7+G7)</f>
         <v>0.0625</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="22" t="s">
         <v>18</v>
       </c>
       <c r="J7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="n">
+      <c r="A8" s="23" t="n">
         <f aca="false">A7+1</f>
         <v>43015</v>
       </c>
-      <c r="B8" s="23" t="n">
+      <c r="B8" s="24" t="n">
         <f aca="false">A8</f>
         <v>43015</v>
       </c>
@@ -1122,19 +1146,19 @@
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16" t="n">
+      <c r="G8" s="17"/>
+      <c r="H8" s="17" t="n">
         <f aca="false">(E8-D8-F8+G8)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="24"/>
+      <c r="I8" s="25"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="n">
+      <c r="A9" s="23" t="n">
         <f aca="false">A8+1</f>
         <v>43016</v>
       </c>
-      <c r="B9" s="23" t="n">
+      <c r="B9" s="24" t="n">
         <f aca="false">A9</f>
         <v>43016</v>
       </c>
@@ -1145,19 +1169,19 @@
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16" t="n">
+      <c r="G9" s="17"/>
+      <c r="H9" s="17" t="n">
         <f aca="false">(E9-D9-F9+G9)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="24"/>
+      <c r="I9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="n">
+      <c r="A10" s="23" t="n">
         <f aca="false">A9+1</f>
         <v>43017</v>
       </c>
-      <c r="B10" s="23" t="n">
+      <c r="B10" s="24" t="n">
         <f aca="false">A10</f>
         <v>43017</v>
       </c>
@@ -1168,18 +1192,18 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16" t="n">
+      <c r="G10" s="17"/>
+      <c r="H10" s="17" t="n">
         <f aca="false">(E10-D10-F10+G10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="n">
+      <c r="A11" s="23" t="n">
         <f aca="false">A10+1</f>
         <v>43018</v>
       </c>
-      <c r="B11" s="23" t="n">
+      <c r="B11" s="24" t="n">
         <f aca="false">A11</f>
         <v>43018</v>
       </c>
@@ -1190,18 +1214,18 @@
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16" t="n">
+      <c r="G11" s="17"/>
+      <c r="H11" s="17" t="n">
         <f aca="false">(E11-D11-F11+G11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="n">
+      <c r="A12" s="23" t="n">
         <f aca="false">A11+1</f>
         <v>43019</v>
       </c>
-      <c r="B12" s="23" t="n">
+      <c r="B12" s="24" t="n">
         <f aca="false">A12</f>
         <v>43019</v>
       </c>
@@ -1212,18 +1236,18 @@
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16" t="n">
+      <c r="G12" s="17"/>
+      <c r="H12" s="17" t="n">
         <f aca="false">(E12-D12-F12+G12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="n">
+      <c r="A13" s="23" t="n">
         <f aca="false">A12+1</f>
         <v>43020</v>
       </c>
-      <c r="B13" s="23" t="n">
+      <c r="B13" s="24" t="n">
         <f aca="false">A13</f>
         <v>43020</v>
       </c>
@@ -1234,18 +1258,18 @@
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16" t="n">
+      <c r="G13" s="17"/>
+      <c r="H13" s="17" t="n">
         <f aca="false">(E13-D13-F13+G13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="25" t="n">
+      <c r="A14" s="26" t="n">
         <f aca="false">A13+1</f>
         <v>43021</v>
       </c>
-      <c r="B14" s="26" t="n">
+      <c r="B14" s="27" t="n">
         <f aca="false">A14</f>
         <v>43021</v>
       </c>
@@ -1256,27 +1280,27 @@
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="16" t="n">
+      <c r="G14" s="17" t="n">
         <v>0.0833333333333333</v>
       </c>
-      <c r="H14" s="16" t="n">
+      <c r="H14" s="17" t="n">
         <f aca="false">(E14-D14-F14+G14)</f>
         <v>0.0833333333333333</v>
       </c>
-      <c r="I14" s="27" t="s">
+      <c r="I14" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="29"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22" t="n">
+      <c r="A15" s="23" t="n">
         <f aca="false">A14+1</f>
         <v>43022</v>
       </c>
-      <c r="B15" s="23" t="n">
+      <c r="B15" s="24" t="n">
         <f aca="false">A15</f>
         <v>43022</v>
       </c>
@@ -1287,19 +1311,19 @@
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16" t="n">
+      <c r="G15" s="17"/>
+      <c r="H15" s="17" t="n">
         <f aca="false">(E15-D15-F15+G15)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="24"/>
+      <c r="I15" s="25"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22" t="n">
+      <c r="A16" s="23" t="n">
         <f aca="false">A15+1</f>
         <v>43023</v>
       </c>
-      <c r="B16" s="23" t="n">
+      <c r="B16" s="24" t="n">
         <f aca="false">A16</f>
         <v>43023</v>
       </c>
@@ -1310,19 +1334,19 @@
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16" t="n">
+      <c r="G16" s="17"/>
+      <c r="H16" s="17" t="n">
         <f aca="false">(E16-D16-F16+G16)</f>
         <v>0</v>
       </c>
-      <c r="I16" s="24"/>
+      <c r="I16" s="25"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22" t="n">
+      <c r="A17" s="23" t="n">
         <f aca="false">A16+1</f>
         <v>43024</v>
       </c>
-      <c r="B17" s="23" t="n">
+      <c r="B17" s="24" t="n">
         <f aca="false">A17</f>
         <v>43024</v>
       </c>
@@ -1333,19 +1357,19 @@
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16" t="n">
+      <c r="G17" s="17"/>
+      <c r="H17" s="17" t="n">
         <f aca="false">(E17-D17-F17+G17)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="24"/>
+      <c r="I17" s="25"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22" t="n">
+      <c r="A18" s="23" t="n">
         <f aca="false">A17+1</f>
         <v>43025</v>
       </c>
-      <c r="B18" s="23" t="n">
+      <c r="B18" s="24" t="n">
         <f aca="false">A18</f>
         <v>43025</v>
       </c>
@@ -1356,8 +1380,8 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16" t="n">
+      <c r="G18" s="17"/>
+      <c r="H18" s="17" t="n">
         <f aca="false">(E18-D18-F18+G18)</f>
         <v>0</v>
       </c>
@@ -1366,11 +1390,11 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="n">
+      <c r="A19" s="23" t="n">
         <f aca="false">A18+1</f>
         <v>43026</v>
       </c>
-      <c r="B19" s="23" t="n">
+      <c r="B19" s="24" t="n">
         <f aca="false">A19</f>
         <v>43026</v>
       </c>
@@ -1381,18 +1405,18 @@
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16" t="n">
+      <c r="G19" s="17"/>
+      <c r="H19" s="17" t="n">
         <f aca="false">(E19-D19-F19+G19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22" t="n">
+      <c r="A20" s="23" t="n">
         <f aca="false">A19+1</f>
         <v>43027</v>
       </c>
-      <c r="B20" s="23" t="n">
+      <c r="B20" s="24" t="n">
         <f aca="false">A20</f>
         <v>43027</v>
       </c>
@@ -1409,18 +1433,21 @@
       <c r="F20" s="9" t="n">
         <v>0.125</v>
       </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16" t="n">
+      <c r="G20" s="17"/>
+      <c r="H20" s="17" t="n">
         <f aca="false">(E20-D20-F20+G20)</f>
         <v>0.172916666666667</v>
       </c>
+      <c r="I20" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="21" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="25" t="n">
+      <c r="A21" s="26" t="n">
         <f aca="false">A20+1</f>
         <v>43028</v>
       </c>
-      <c r="B21" s="26" t="n">
+      <c r="B21" s="27" t="n">
         <f aca="false">A21</f>
         <v>43028</v>
       </c>
@@ -1437,27 +1464,27 @@
       <c r="F21" s="9" t="n">
         <v>0.104166666666667</v>
       </c>
-      <c r="G21" s="16" t="n">
+      <c r="G21" s="17" t="n">
         <v>0.0833333333333333</v>
       </c>
-      <c r="H21" s="16" t="n">
+      <c r="H21" s="17" t="n">
         <f aca="false">(E21-D21-F21+G21)</f>
         <v>0.184027777777778</v>
       </c>
-      <c r="I21" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
+      <c r="I21" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="22" t="n">
+      <c r="A22" s="23" t="n">
         <f aca="false">A21+1</f>
         <v>43029</v>
       </c>
-      <c r="B22" s="23" t="n">
+      <c r="B22" s="24" t="n">
         <f aca="false">A22</f>
         <v>43029</v>
       </c>
@@ -1468,19 +1495,19 @@
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16" t="n">
+      <c r="G22" s="17"/>
+      <c r="H22" s="17" t="n">
         <f aca="false">(E22-D22-F22+G22)</f>
         <v>0</v>
       </c>
-      <c r="I22" s="24"/>
+      <c r="I22" s="25"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="22" t="n">
+      <c r="A23" s="23" t="n">
         <f aca="false">A22+1</f>
         <v>43030</v>
       </c>
-      <c r="B23" s="23" t="n">
+      <c r="B23" s="24" t="n">
         <f aca="false">A23</f>
         <v>43030</v>
       </c>
@@ -1491,19 +1518,19 @@
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16" t="n">
+      <c r="G23" s="17"/>
+      <c r="H23" s="17" t="n">
         <f aca="false">(E23-D23-F23+G23)</f>
         <v>0</v>
       </c>
-      <c r="I23" s="24"/>
+      <c r="I23" s="25"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="n">
+      <c r="A24" s="23" t="n">
         <f aca="false">A23+1</f>
         <v>43031</v>
       </c>
-      <c r="B24" s="23" t="n">
+      <c r="B24" s="24" t="n">
         <f aca="false">A24</f>
         <v>43031</v>
       </c>
@@ -1514,18 +1541,18 @@
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16" t="n">
+      <c r="G24" s="17"/>
+      <c r="H24" s="17" t="n">
         <f aca="false">(E24-D24-F24+G24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="n">
+      <c r="A25" s="23" t="n">
         <f aca="false">A24+1</f>
         <v>43032</v>
       </c>
-      <c r="B25" s="23" t="n">
+      <c r="B25" s="24" t="n">
         <f aca="false">A25</f>
         <v>43032</v>
       </c>
@@ -1536,18 +1563,18 @@
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16" t="n">
+      <c r="G25" s="17"/>
+      <c r="H25" s="17" t="n">
         <f aca="false">(E25-D25-F25+G25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22" t="n">
+      <c r="A26" s="23" t="n">
         <f aca="false">A25+1</f>
         <v>43033</v>
       </c>
-      <c r="B26" s="23" t="n">
+      <c r="B26" s="24" t="n">
         <f aca="false">A26</f>
         <v>43033</v>
       </c>
@@ -1558,18 +1585,18 @@
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16" t="n">
+      <c r="G26" s="17"/>
+      <c r="H26" s="17" t="n">
         <f aca="false">(E26-D26-F26+G26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22" t="n">
+      <c r="A27" s="23" t="n">
         <f aca="false">A26+1</f>
         <v>43034</v>
       </c>
-      <c r="B27" s="23" t="n">
+      <c r="B27" s="24" t="n">
         <f aca="false">A27</f>
         <v>43034</v>
       </c>
@@ -1580,18 +1607,18 @@
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16" t="n">
+      <c r="G27" s="17"/>
+      <c r="H27" s="17" t="n">
         <f aca="false">(E27-D27-F27+G27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="22" t="n">
+      <c r="A28" s="23" t="n">
         <f aca="false">A27+1</f>
         <v>43035</v>
       </c>
-      <c r="B28" s="23" t="n">
+      <c r="B28" s="24" t="n">
         <f aca="false">A28</f>
         <v>43035</v>
       </c>
@@ -1602,23 +1629,23 @@
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="16" t="n">
+      <c r="G28" s="17" t="n">
         <v>0.0833333333333333</v>
       </c>
-      <c r="H28" s="16" t="n">
+      <c r="H28" s="17" t="n">
         <f aca="false">(E28-D28-F28+G28)</f>
         <v>0.0833333333333333</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="22" t="n">
+      <c r="A29" s="23" t="n">
         <f aca="false">A28+1</f>
         <v>43036</v>
       </c>
-      <c r="B29" s="23" t="n">
+      <c r="B29" s="24" t="n">
         <f aca="false">A29</f>
         <v>43036</v>
       </c>
@@ -1629,19 +1656,19 @@
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16" t="n">
+      <c r="G29" s="17"/>
+      <c r="H29" s="17" t="n">
         <f aca="false">(E29-D29-F29+G29)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="24"/>
+      <c r="I29" s="25"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="22" t="n">
+      <c r="A30" s="23" t="n">
         <f aca="false">A29+1</f>
         <v>43037</v>
       </c>
-      <c r="B30" s="23" t="n">
+      <c r="B30" s="24" t="n">
         <f aca="false">A30</f>
         <v>43037</v>
       </c>
@@ -1656,21 +1683,21 @@
         <v>0.722916666666667</v>
       </c>
       <c r="F30" s="9"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16" t="n">
+      <c r="G30" s="17"/>
+      <c r="H30" s="17" t="n">
         <f aca="false">(E30-D30-F30+G30)</f>
         <v>0.090972222222223</v>
       </c>
-      <c r="I30" s="30" t="s">
-        <v>23</v>
+      <c r="I30" s="31" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="22" t="n">
+      <c r="A31" s="23" t="n">
         <f aca="false">A30+1</f>
         <v>43038</v>
       </c>
-      <c r="B31" s="23" t="n">
+      <c r="B31" s="24" t="n">
         <f aca="false">A31</f>
         <v>43038</v>
       </c>
@@ -1681,40 +1708,40 @@
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16" t="n">
+      <c r="G31" s="17"/>
+      <c r="H31" s="17" t="n">
         <f aca="false">(E31-D31-F31+G31)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="31" t="n">
+      <c r="A32" s="32" t="n">
         <f aca="false">A31+1</f>
         <v>43039</v>
       </c>
-      <c r="B32" s="32" t="n">
+      <c r="B32" s="33" t="n">
         <f aca="false">A32</f>
         <v>43039</v>
       </c>
-      <c r="C32" s="33" t="n">
+      <c r="C32" s="34" t="n">
         <f aca="false">WEEKNUM(A32,2)</f>
         <v>45</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="16" t="n">
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="17" t="n">
         <f aca="false">(E32-D32-F32+G32)</f>
         <v>0</v>
       </c>
-      <c r="I32" s="35"/>
+      <c r="I32" s="36"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="36"/>
+      <c r="A33" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="37"/>
       <c r="C33" s="9" t="n">
         <f aca="false">Zusammenfassung!C7</f>
         <v>1.125</v>
@@ -1723,23 +1750,23 @@
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="37"/>
+      <c r="H33" s="38"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40" t="n">
+      <c r="A34" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="39"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41" t="n">
         <f aca="false">SUM(H2:H32)</f>
         <v>0.677083333333334</v>
       </c>
-      <c r="I34" s="41"/>
+      <c r="I34" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1823,8 +1850,8 @@
   </sheetPr>
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L23" activeCellId="0" sqref="L23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1832,7 +1859,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.57"/>
@@ -1840,40 +1867,40 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="42" t="n">
+      <c r="A2" s="43" t="n">
         <f aca="false">DATE(2017,11,1)</f>
         <v>43040</v>
       </c>
-      <c r="B2" s="23" t="n">
+      <c r="B2" s="24" t="n">
         <f aca="false">A2</f>
         <v>43040</v>
       </c>
@@ -1891,11 +1918,11 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42" t="n">
+      <c r="A3" s="43" t="n">
         <f aca="false">A2+1</f>
         <v>43041</v>
       </c>
-      <c r="B3" s="23" t="n">
+      <c r="B3" s="24" t="n">
         <f aca="false">A3</f>
         <v>43041</v>
       </c>
@@ -1913,11 +1940,11 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="42" t="n">
+      <c r="A4" s="43" t="n">
         <f aca="false">A3+1</f>
         <v>43042</v>
       </c>
-      <c r="B4" s="23" t="n">
+      <c r="B4" s="24" t="n">
         <f aca="false">A4</f>
         <v>43042</v>
       </c>
@@ -1936,15 +1963,15 @@
         <v>0.0833333333333333</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="42" t="n">
+      <c r="A5" s="43" t="n">
         <f aca="false">A4+1</f>
         <v>43043</v>
       </c>
-      <c r="B5" s="23" t="n">
+      <c r="B5" s="24" t="n">
         <f aca="false">A5</f>
         <v>43043</v>
       </c>
@@ -1964,16 +1991,16 @@
         <f aca="false">(E5-D5-F5+G5)</f>
         <v>0.1125</v>
       </c>
-      <c r="I5" s="43" t="s">
-        <v>27</v>
+      <c r="I5" s="44" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="42" t="n">
+      <c r="A6" s="43" t="n">
         <f aca="false">A5+1</f>
         <v>43044</v>
       </c>
-      <c r="B6" s="23" t="n">
+      <c r="B6" s="24" t="n">
         <f aca="false">A6</f>
         <v>43044</v>
       </c>
@@ -1989,14 +2016,14 @@
         <f aca="false">(E6-D6-F6+G6)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="24"/>
+      <c r="I6" s="25"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="42" t="n">
+      <c r="A7" s="43" t="n">
         <f aca="false">A6+1</f>
         <v>43045</v>
       </c>
-      <c r="B7" s="23" t="n">
+      <c r="B7" s="24" t="n">
         <f aca="false">A7</f>
         <v>43045</v>
       </c>
@@ -2014,11 +2041,11 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="42" t="n">
+      <c r="A8" s="43" t="n">
         <f aca="false">A7+1</f>
         <v>43046</v>
       </c>
-      <c r="B8" s="23" t="n">
+      <c r="B8" s="24" t="n">
         <f aca="false">A8</f>
         <v>43046</v>
       </c>
@@ -2039,15 +2066,15 @@
         <v>0.0729166666666666</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="42" t="n">
+      <c r="A9" s="43" t="n">
         <f aca="false">A8+1</f>
         <v>43047</v>
       </c>
-      <c r="B9" s="23" t="n">
+      <c r="B9" s="24" t="n">
         <f aca="false">A9</f>
         <v>43047</v>
       </c>
@@ -2070,15 +2097,15 @@
         <v>0.134027777777777</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="42" t="n">
+      <c r="A10" s="43" t="n">
         <f aca="false">A9+1</f>
         <v>43048</v>
       </c>
-      <c r="B10" s="23" t="n">
+      <c r="B10" s="24" t="n">
         <f aca="false">A10</f>
         <v>43048</v>
       </c>
@@ -2096,11 +2123,11 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="42" t="n">
+      <c r="A11" s="43" t="n">
         <f aca="false">A10+1</f>
         <v>43049</v>
       </c>
-      <c r="B11" s="23" t="n">
+      <c r="B11" s="24" t="n">
         <f aca="false">A11</f>
         <v>43049</v>
       </c>
@@ -2120,11 +2147,11 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="42" t="n">
+      <c r="A12" s="43" t="n">
         <f aca="false">A11+1</f>
         <v>43050</v>
       </c>
-      <c r="B12" s="23" t="n">
+      <c r="B12" s="24" t="n">
         <f aca="false">A12</f>
         <v>43050</v>
       </c>
@@ -2140,14 +2167,14 @@
         <f aca="false">(E12-D12-F12+G12)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="24"/>
+      <c r="I12" s="25"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="42" t="n">
+      <c r="A13" s="43" t="n">
         <f aca="false">A12+1</f>
         <v>43051</v>
       </c>
-      <c r="B13" s="23" t="n">
+      <c r="B13" s="24" t="n">
         <f aca="false">A13</f>
         <v>43051</v>
       </c>
@@ -2163,14 +2190,14 @@
         <f aca="false">(E13-D13-F13+G13)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="24"/>
+      <c r="I13" s="25"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="42" t="n">
+      <c r="A14" s="43" t="n">
         <f aca="false">A13+1</f>
         <v>43052</v>
       </c>
-      <c r="B14" s="23" t="n">
+      <c r="B14" s="24" t="n">
         <f aca="false">A14</f>
         <v>43052</v>
       </c>
@@ -2193,15 +2220,15 @@
         <v>0.0625</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="42" t="n">
+      <c r="A15" s="43" t="n">
         <f aca="false">A14+1</f>
         <v>43053</v>
       </c>
-      <c r="B15" s="23" t="n">
+      <c r="B15" s="24" t="n">
         <f aca="false">A15</f>
         <v>43053</v>
       </c>
@@ -2224,15 +2251,15 @@
         <v>0.14375</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="42" t="n">
+      <c r="A16" s="43" t="n">
         <f aca="false">A15+1</f>
         <v>43054</v>
       </c>
-      <c r="B16" s="23" t="n">
+      <c r="B16" s="24" t="n">
         <f aca="false">A16</f>
         <v>43054</v>
       </c>
@@ -2255,15 +2282,15 @@
         <v>0.133333333333333</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="42" t="n">
+      <c r="A17" s="43" t="n">
         <f aca="false">A16+1</f>
         <v>43055</v>
       </c>
-      <c r="B17" s="23" t="n">
+      <c r="B17" s="24" t="n">
         <f aca="false">A17</f>
         <v>43055</v>
       </c>
@@ -2284,15 +2311,15 @@
         <v>0.0833333333333333</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="44" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="45" t="n">
         <f aca="false">A17+1</f>
         <v>43056</v>
       </c>
-      <c r="B18" s="26" t="n">
+      <c r="B18" s="27" t="n">
         <f aca="false">A18</f>
         <v>43056</v>
       </c>
@@ -2303,24 +2330,26 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="G18" s="9" t="n">
+        <v>0.0416666666666667</v>
+      </c>
       <c r="H18" s="9" t="n">
         <f aca="false">(E18-D18-F18+G18)</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="42" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="43" t="n">
         <f aca="false">A18+1</f>
         <v>43057</v>
       </c>
-      <c r="B19" s="23" t="n">
+      <c r="B19" s="24" t="n">
         <f aca="false">A19</f>
         <v>43057</v>
       </c>
@@ -2328,21 +2357,28 @@
         <f aca="false">WEEKNUM(A19,2)</f>
         <v>47</v>
       </c>
-      <c r="G19" s="9" t="n">
-        <v>0.0416666666666667</v>
-      </c>
+      <c r="D19" s="9" t="n">
+        <v>0.631944444444444</v>
+      </c>
+      <c r="E19" s="9" t="n">
+        <v>0.729166666666667</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="9" t="n">
         <f aca="false">(E19-D19-F19+G19)</f>
-        <v>0.0416666666666667</v>
-      </c>
-      <c r="I19" s="24"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="42" t="n">
+        <v>0.0972222222222222</v>
+      </c>
+      <c r="I19" s="44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="43" t="n">
         <f aca="false">A19+1</f>
         <v>43058</v>
       </c>
-      <c r="B20" s="23" t="n">
+      <c r="B20" s="24" t="n">
         <f aca="false">A20</f>
         <v>43058</v>
       </c>
@@ -2360,17 +2396,20 @@
         <v>0.03125</v>
       </c>
       <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="43" t="s">
-        <v>35</v>
+      <c r="H20" s="9" t="n">
+        <f aca="false">(E20-D20-F20+G20)</f>
+        <v>0.14375</v>
+      </c>
+      <c r="I20" s="44" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="42" t="n">
+      <c r="A21" s="43" t="n">
         <f aca="false">A20+1</f>
         <v>43059</v>
       </c>
-      <c r="B21" s="23" t="n">
+      <c r="B21" s="24" t="n">
         <f aca="false">A21</f>
         <v>43059</v>
       </c>
@@ -2388,11 +2427,11 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="42" t="n">
+      <c r="A22" s="43" t="n">
         <f aca="false">A21+1</f>
         <v>43060</v>
       </c>
-      <c r="B22" s="23" t="n">
+      <c r="B22" s="24" t="n">
         <f aca="false">A22</f>
         <v>43060</v>
       </c>
@@ -2410,11 +2449,11 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="42" t="n">
+      <c r="A23" s="43" t="n">
         <f aca="false">A22+1</f>
         <v>43061</v>
       </c>
-      <c r="B23" s="23" t="n">
+      <c r="B23" s="24" t="n">
         <f aca="false">A23</f>
         <v>43061</v>
       </c>
@@ -2437,15 +2476,15 @@
         <v>0.145833333333333</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="42" t="n">
+      <c r="A24" s="43" t="n">
         <f aca="false">A23+1</f>
         <v>43062</v>
       </c>
-      <c r="B24" s="23" t="n">
+      <c r="B24" s="24" t="n">
         <f aca="false">A24</f>
         <v>43062</v>
       </c>
@@ -2463,11 +2502,11 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="42" t="n">
+      <c r="A25" s="43" t="n">
         <f aca="false">A24+1</f>
         <v>43063</v>
       </c>
-      <c r="B25" s="23" t="n">
+      <c r="B25" s="24" t="n">
         <f aca="false">A25</f>
         <v>43063</v>
       </c>
@@ -2492,15 +2531,15 @@
         <v>0.211111111111111</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="42" t="n">
+      <c r="A26" s="43" t="n">
         <f aca="false">A25+1</f>
         <v>43064</v>
       </c>
-      <c r="B26" s="23" t="n">
+      <c r="B26" s="24" t="n">
         <f aca="false">A26</f>
         <v>43064</v>
       </c>
@@ -2516,14 +2555,14 @@
         <f aca="false">(E26-D26-F26+G26)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="24"/>
+      <c r="I26" s="25"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="42" t="n">
+      <c r="A27" s="43" t="n">
         <f aca="false">A26+1</f>
         <v>43065</v>
       </c>
-      <c r="B27" s="23" t="n">
+      <c r="B27" s="24" t="n">
         <f aca="false">A27</f>
         <v>43065</v>
       </c>
@@ -2539,14 +2578,14 @@
         <f aca="false">(E27-D27-F27+G27)</f>
         <v>0</v>
       </c>
-      <c r="I27" s="24"/>
+      <c r="I27" s="25"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="42" t="n">
+      <c r="A28" s="43" t="n">
         <f aca="false">A27+1</f>
         <v>43066</v>
       </c>
-      <c r="B28" s="23" t="n">
+      <c r="B28" s="24" t="n">
         <f aca="false">A28</f>
         <v>43066</v>
       </c>
@@ -2569,15 +2608,15 @@
         <v>0.190277777777778</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="42" t="n">
+      <c r="A29" s="43" t="n">
         <f aca="false">A28+1</f>
         <v>43067</v>
       </c>
-      <c r="B29" s="23" t="n">
+      <c r="B29" s="24" t="n">
         <f aca="false">A29</f>
         <v>43067</v>
       </c>
@@ -2595,11 +2634,11 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="42" t="n">
+      <c r="A30" s="43" t="n">
         <f aca="false">A29+1</f>
         <v>43068</v>
       </c>
-      <c r="B30" s="23" t="n">
+      <c r="B30" s="24" t="n">
         <f aca="false">A30</f>
         <v>43068</v>
       </c>
@@ -2622,15 +2661,15 @@
         <v>0.208333333333333</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="42" t="n">
+      <c r="A31" s="43" t="n">
         <f aca="false">A30+1</f>
         <v>43069</v>
       </c>
-      <c r="B31" s="23" t="n">
+      <c r="B31" s="24" t="n">
         <f aca="false">A31</f>
         <v>43069</v>
       </c>
@@ -2651,25 +2690,25 @@
         <v>0.0972222222222222</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="45"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="35"/>
+      <c r="A32" s="46"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="36"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="36"/>
+      <c r="A33" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="37"/>
       <c r="C33" s="9" t="n">
         <f aca="false">Zusammenfassung!C8</f>
         <v>1.875</v>
@@ -2681,20 +2720,20 @@
       <c r="H33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40" t="n">
+      <c r="A34" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="39"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41" t="n">
         <f aca="false">SUM(H2:H32)</f>
-        <v>1.80347222222222</v>
-      </c>
-      <c r="I34" s="41"/>
+        <v>2.04444444444444</v>
+      </c>
+      <c r="I34" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2767,8 +2806,8 @@
   </sheetPr>
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2784,40 +2823,40 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="42" t="n">
+      <c r="A2" s="43" t="n">
         <f aca="false">DATE(2017,12,1)</f>
         <v>43070</v>
       </c>
-      <c r="B2" s="23" t="n">
+      <c r="B2" s="24" t="n">
         <f aca="false">A2</f>
         <v>43070</v>
       </c>
@@ -2825,32 +2864,32 @@
         <f aca="false">WEEKNUM(A2,2)</f>
         <v>49</v>
       </c>
-      <c r="D2" s="46" t="n">
+      <c r="D2" s="47" t="n">
         <v>0.634722222222222</v>
       </c>
-      <c r="E2" s="46" t="n">
+      <c r="E2" s="47" t="n">
         <v>0.791666666666667</v>
       </c>
-      <c r="F2" s="46" t="n">
+      <c r="F2" s="47" t="n">
         <v>0.0416666666666667</v>
       </c>
-      <c r="G2" s="46" t="n">
+      <c r="G2" s="47" t="n">
         <v>0.125</v>
       </c>
-      <c r="H2" s="47" t="n">
+      <c r="H2" s="48" t="n">
         <f aca="false">(E2-D2-F2+G2)</f>
         <v>0.240277777777778</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42" t="n">
+      <c r="A3" s="43" t="n">
         <f aca="false">A2+1</f>
         <v>43071</v>
       </c>
-      <c r="B3" s="23" t="n">
+      <c r="B3" s="24" t="n">
         <f aca="false">A3</f>
         <v>43071</v>
       </c>
@@ -2858,30 +2897,30 @@
         <f aca="false">WEEKNUM(A3,2)</f>
         <v>49</v>
       </c>
-      <c r="D3" s="46" t="n">
+      <c r="D3" s="47" t="n">
         <v>0.645833333333333</v>
       </c>
-      <c r="E3" s="46" t="n">
+      <c r="E3" s="47" t="n">
         <v>0.846527777777778</v>
       </c>
-      <c r="F3" s="46" t="n">
+      <c r="F3" s="47" t="n">
         <v>0.0625</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="47" t="n">
+      <c r="G3" s="47"/>
+      <c r="H3" s="48" t="n">
         <f aca="false">(E3-D3-F3+G3)</f>
         <v>0.138194444444444</v>
       </c>
-      <c r="I3" s="43" t="s">
-        <v>42</v>
+      <c r="I3" s="44" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="42" t="n">
+      <c r="A4" s="43" t="n">
         <f aca="false">A3+1</f>
         <v>43072</v>
       </c>
-      <c r="B4" s="23" t="n">
+      <c r="B4" s="24" t="n">
         <f aca="false">A4</f>
         <v>43072</v>
       </c>
@@ -2889,28 +2928,28 @@
         <f aca="false">WEEKNUM(A4,2)</f>
         <v>49</v>
       </c>
-      <c r="D4" s="46" t="n">
+      <c r="D4" s="47" t="n">
         <v>0.729166666666667</v>
       </c>
-      <c r="E4" s="46" t="n">
+      <c r="E4" s="47" t="n">
         <v>0.805555555555556</v>
       </c>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="47" t="n">
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="48" t="n">
         <f aca="false">(E4-D4-F4+G4)</f>
         <v>0.0763888888888889</v>
       </c>
-      <c r="I4" s="24" t="s">
-        <v>43</v>
+      <c r="I4" s="25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="42" t="n">
+      <c r="A5" s="43" t="n">
         <f aca="false">A4+1</f>
         <v>43073</v>
       </c>
-      <c r="B5" s="23" t="n">
+      <c r="B5" s="24" t="n">
         <f aca="false">A5</f>
         <v>43073</v>
       </c>
@@ -2918,21 +2957,21 @@
         <f aca="false">WEEKNUM(A5,2)</f>
         <v>50</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="47" t="n">
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="48" t="n">
         <f aca="false">(E5-D5-F5+G5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="42" t="n">
+      <c r="A6" s="43" t="n">
         <f aca="false">A5+1</f>
         <v>43074</v>
       </c>
-      <c r="B6" s="23" t="n">
+      <c r="B6" s="24" t="n">
         <f aca="false">A6</f>
         <v>43074</v>
       </c>
@@ -2940,21 +2979,21 @@
         <f aca="false">WEEKNUM(A6,2)</f>
         <v>50</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="47" t="n">
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="48" t="n">
         <f aca="false">(E6-D6-F6+G6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="42" t="n">
+      <c r="A7" s="43" t="n">
         <f aca="false">A6+1</f>
         <v>43075</v>
       </c>
-      <c r="B7" s="23" t="n">
+      <c r="B7" s="24" t="n">
         <f aca="false">A7</f>
         <v>43075</v>
       </c>
@@ -2962,28 +3001,28 @@
         <f aca="false">WEEKNUM(A7,2)</f>
         <v>50</v>
       </c>
-      <c r="D7" s="46" t="n">
+      <c r="D7" s="47" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="E7" s="46" t="n">
+      <c r="E7" s="47" t="n">
         <v>0.479166666666667</v>
       </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="47" t="n">
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="48" t="n">
         <f aca="false">(E7-D7-F7+G7)</f>
         <v>0.0833333333333334</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="42" t="n">
+      <c r="A8" s="43" t="n">
         <f aca="false">A7+1</f>
         <v>43076</v>
       </c>
-      <c r="B8" s="23" t="n">
+      <c r="B8" s="24" t="n">
         <f aca="false">A8</f>
         <v>43076</v>
       </c>
@@ -2991,28 +3030,28 @@
         <f aca="false">WEEKNUM(A8,2)</f>
         <v>50</v>
       </c>
-      <c r="D8" s="46" t="n">
+      <c r="D8" s="47" t="n">
         <v>0.770833333333333</v>
       </c>
-      <c r="E8" s="46" t="n">
+      <c r="E8" s="47" t="n">
         <v>0.967361111111111</v>
       </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="47" t="n">
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="48" t="n">
         <f aca="false">(E8-D8-F8+G8)</f>
         <v>0.196527777777778</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="42" t="n">
+      <c r="A9" s="43" t="n">
         <f aca="false">A8+1</f>
         <v>43077</v>
       </c>
-      <c r="B9" s="23" t="n">
+      <c r="B9" s="24" t="n">
         <f aca="false">A9</f>
         <v>43077</v>
       </c>
@@ -3020,30 +3059,30 @@
         <f aca="false">WEEKNUM(A9,2)</f>
         <v>50</v>
       </c>
-      <c r="D9" s="46" t="n">
+      <c r="D9" s="47" t="n">
         <v>0.104166666666667</v>
       </c>
-      <c r="E9" s="46" t="n">
+      <c r="E9" s="47" t="n">
         <v>0.900694444444444</v>
       </c>
-      <c r="F9" s="46" t="n">
+      <c r="F9" s="47" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="G9" s="46"/>
-      <c r="H9" s="47" t="n">
+      <c r="G9" s="47"/>
+      <c r="H9" s="48" t="n">
         <f aca="false">(E9-D9-F9+G9)</f>
         <v>0.338194444444444</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="42" t="n">
+      <c r="A10" s="43" t="n">
         <f aca="false">A9+1</f>
         <v>43078</v>
       </c>
-      <c r="B10" s="23" t="n">
+      <c r="B10" s="24" t="n">
         <f aca="false">A10</f>
         <v>43078</v>
       </c>
@@ -3051,30 +3090,30 @@
         <f aca="false">WEEKNUM(A10,2)</f>
         <v>50</v>
       </c>
-      <c r="D10" s="46" t="n">
+      <c r="D10" s="47" t="n">
         <v>0.5625</v>
       </c>
-      <c r="E10" s="46" t="n">
+      <c r="E10" s="47" t="n">
         <v>0.931944444444444</v>
       </c>
-      <c r="F10" s="46" t="n">
+      <c r="F10" s="47" t="n">
         <v>0.125</v>
       </c>
-      <c r="G10" s="46"/>
-      <c r="H10" s="47" t="n">
+      <c r="G10" s="47"/>
+      <c r="H10" s="48" t="n">
         <f aca="false">(E10-D10-F10+G10)</f>
         <v>0.244444444444444</v>
       </c>
-      <c r="I10" s="24" t="s">
-        <v>47</v>
+      <c r="I10" s="25" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="42" t="n">
+      <c r="A11" s="43" t="n">
         <f aca="false">A10+1</f>
         <v>43079</v>
       </c>
-      <c r="B11" s="23" t="n">
+      <c r="B11" s="24" t="n">
         <f aca="false">A11</f>
         <v>43079</v>
       </c>
@@ -3082,28 +3121,28 @@
         <f aca="false">WEEKNUM(A11,2)</f>
         <v>50</v>
       </c>
-      <c r="D11" s="46" t="n">
+      <c r="D11" s="47" t="n">
         <v>0.756944444444444</v>
       </c>
-      <c r="E11" s="46" t="n">
+      <c r="E11" s="47" t="n">
         <v>0.847222222222222</v>
       </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="47" t="n">
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="48" t="n">
         <f aca="false">(E11-D11-F11+G11)</f>
         <v>0.0902777777777778</v>
       </c>
-      <c r="I11" s="43" t="s">
-        <v>48</v>
+      <c r="I11" s="44" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="42" t="n">
+      <c r="A12" s="43" t="n">
         <f aca="false">A11+1</f>
         <v>43080</v>
       </c>
-      <c r="B12" s="23" t="n">
+      <c r="B12" s="24" t="n">
         <f aca="false">A12</f>
         <v>43080</v>
       </c>
@@ -3111,30 +3150,30 @@
         <f aca="false">WEEKNUM(A12,2)</f>
         <v>51</v>
       </c>
-      <c r="D12" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="46" t="n">
+      <c r="D12" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="47" t="n">
         <v>0.125</v>
       </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46" t="n">
+      <c r="F12" s="47"/>
+      <c r="G12" s="47" t="n">
         <v>0.25</v>
       </c>
-      <c r="H12" s="47" t="n">
+      <c r="H12" s="48" t="n">
         <f aca="false">(E12-D12-F12+G12)</f>
         <v>0.375</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="42" t="n">
+      <c r="A13" s="43" t="n">
         <f aca="false">A12+1</f>
         <v>43081</v>
       </c>
-      <c r="B13" s="23" t="n">
+      <c r="B13" s="24" t="n">
         <f aca="false">A13</f>
         <v>43081</v>
       </c>
@@ -3142,30 +3181,30 @@
         <f aca="false">WEEKNUM(A13,2)</f>
         <v>51</v>
       </c>
-      <c r="D13" s="46" t="n">
+      <c r="D13" s="47" t="n">
         <v>0.770833333333333</v>
       </c>
-      <c r="E13" s="46" t="n">
+      <c r="E13" s="47" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46" t="n">
+      <c r="F13" s="47"/>
+      <c r="G13" s="47" t="n">
         <v>0.1875</v>
       </c>
-      <c r="H13" s="47" t="n">
+      <c r="H13" s="48" t="n">
         <f aca="false">(E13-D13-F13+G13)</f>
         <v>0.416666666666667</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="42" t="n">
+      <c r="A14" s="43" t="n">
         <f aca="false">A13+1</f>
         <v>43082</v>
       </c>
-      <c r="B14" s="23" t="n">
+      <c r="B14" s="24" t="n">
         <f aca="false">A14</f>
         <v>43082</v>
       </c>
@@ -3173,28 +3212,28 @@
         <f aca="false">WEEKNUM(A14,2)</f>
         <v>51</v>
       </c>
-      <c r="D14" s="46" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="46" t="n">
+      <c r="D14" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="47" t="n">
         <v>0.138194444444444</v>
       </c>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="47" t="n">
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="48" t="n">
         <f aca="false">(E14-D14-F14+G14)</f>
         <v>0.138194444444444</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="42" t="n">
+      <c r="A15" s="43" t="n">
         <f aca="false">A14+1</f>
         <v>43083</v>
       </c>
-      <c r="B15" s="23" t="n">
+      <c r="B15" s="24" t="n">
         <f aca="false">A15</f>
         <v>43083</v>
       </c>
@@ -3202,32 +3241,32 @@
         <f aca="false">WEEKNUM(A15,2)</f>
         <v>51</v>
       </c>
-      <c r="D15" s="46" t="n">
+      <c r="D15" s="47" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="E15" s="46" t="n">
+      <c r="E15" s="47" t="n">
         <v>0.875</v>
       </c>
-      <c r="F15" s="46" t="n">
+      <c r="F15" s="47" t="n">
         <v>0.0416666666666667</v>
       </c>
-      <c r="G15" s="46" t="n">
+      <c r="G15" s="47" t="n">
         <v>0.125</v>
       </c>
-      <c r="H15" s="47" t="n">
+      <c r="H15" s="48" t="n">
         <f aca="false">(E15-D15-F15+G15)</f>
         <v>0.291666666666666</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="44" t="n">
+      <c r="A16" s="45" t="n">
         <f aca="false">A15+1</f>
         <v>43084</v>
       </c>
-      <c r="B16" s="26" t="n">
+      <c r="B16" s="27" t="n">
         <f aca="false">A16</f>
         <v>43084</v>
       </c>
@@ -3238,26 +3277,26 @@
       <c r="D16" s="0"/>
       <c r="E16" s="0"/>
       <c r="F16" s="0"/>
-      <c r="G16" s="46" t="n">
+      <c r="G16" s="47" t="n">
         <v>0.0833333333333333</v>
       </c>
-      <c r="H16" s="47" t="n">
+      <c r="H16" s="48" t="n">
         <f aca="false">(E16-D16-F16+G16)</f>
         <v>0.0833333333333333</v>
       </c>
-      <c r="I16" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
+      <c r="I16" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="42" t="n">
+      <c r="A17" s="43" t="n">
         <f aca="false">A16+1</f>
         <v>43085</v>
       </c>
-      <c r="B17" s="23" t="n">
+      <c r="B17" s="24" t="n">
         <f aca="false">A17</f>
         <v>43085</v>
       </c>
@@ -3265,22 +3304,22 @@
         <f aca="false">WEEKNUM(A17,2)</f>
         <v>51</v>
       </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="47" t="n">
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="48" t="n">
         <f aca="false">(E17-D17-F17+G17)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="24"/>
+      <c r="I17" s="44"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="42" t="n">
+      <c r="A18" s="43" t="n">
         <f aca="false">A17+1</f>
         <v>43086</v>
       </c>
-      <c r="B18" s="23" t="n">
+      <c r="B18" s="24" t="n">
         <f aca="false">A18</f>
         <v>43086</v>
       </c>
@@ -3288,22 +3327,22 @@
         <f aca="false">WEEKNUM(A18,2)</f>
         <v>51</v>
       </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="47" t="n">
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="48" t="n">
         <f aca="false">(E18-D18-F18+G18)</f>
         <v>0</v>
       </c>
-      <c r="I18" s="24"/>
+      <c r="I18" s="25"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="42" t="n">
+      <c r="A19" s="43" t="n">
         <f aca="false">A18+1</f>
         <v>43087</v>
       </c>
-      <c r="B19" s="23" t="n">
+      <c r="B19" s="24" t="n">
         <f aca="false">A19</f>
         <v>43087</v>
       </c>
@@ -3311,21 +3350,21 @@
         <f aca="false">WEEKNUM(A19,2)</f>
         <v>52</v>
       </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="47" t="n">
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="48" t="n">
         <f aca="false">(E19-D19-F19+G19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="42" t="n">
+      <c r="A20" s="43" t="n">
         <f aca="false">A19+1</f>
         <v>43088</v>
       </c>
-      <c r="B20" s="23" t="n">
+      <c r="B20" s="24" t="n">
         <f aca="false">A20</f>
         <v>43088</v>
       </c>
@@ -3333,28 +3372,28 @@
         <f aca="false">WEEKNUM(A20,2)</f>
         <v>52</v>
       </c>
-      <c r="D20" s="46" t="n">
+      <c r="D20" s="47" t="n">
         <v>0.645833333333333</v>
       </c>
-      <c r="E20" s="46" t="n">
+      <c r="E20" s="47" t="n">
         <v>0.6875</v>
       </c>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="47" t="n">
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="48" t="n">
         <f aca="false">(E20-D20-F20+G20)</f>
         <v>0.0416666666666666</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="42" t="n">
+      <c r="A21" s="43" t="n">
         <f aca="false">A20+1</f>
         <v>43089</v>
       </c>
-      <c r="B21" s="23" t="n">
+      <c r="B21" s="24" t="n">
         <f aca="false">A21</f>
         <v>43089</v>
       </c>
@@ -3362,21 +3401,21 @@
         <f aca="false">WEEKNUM(A21,2)</f>
         <v>52</v>
       </c>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="47" t="n">
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="48" t="n">
         <f aca="false">(E21-D21-F21+G21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="42" t="n">
+      <c r="A22" s="43" t="n">
         <f aca="false">A21+1</f>
         <v>43090</v>
       </c>
-      <c r="B22" s="23" t="n">
+      <c r="B22" s="24" t="n">
         <f aca="false">A22</f>
         <v>43090</v>
       </c>
@@ -3384,21 +3423,21 @@
         <f aca="false">WEEKNUM(A22,2)</f>
         <v>52</v>
       </c>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="47" t="n">
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="48" t="n">
         <f aca="false">(E22-D22-F22+G22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="42" t="n">
+      <c r="A23" s="43" t="n">
         <f aca="false">A22+1</f>
         <v>43091</v>
       </c>
-      <c r="B23" s="23" t="n">
+      <c r="B23" s="24" t="n">
         <f aca="false">A23</f>
         <v>43091</v>
       </c>
@@ -3406,21 +3445,21 @@
         <f aca="false">WEEKNUM(A23,2)</f>
         <v>52</v>
       </c>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="47" t="n">
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="48" t="n">
         <f aca="false">(E23-D23-F23+G23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="42" t="n">
+      <c r="A24" s="43" t="n">
         <f aca="false">A23+1</f>
         <v>43092</v>
       </c>
-      <c r="B24" s="23" t="n">
+      <c r="B24" s="24" t="n">
         <f aca="false">A24</f>
         <v>43092</v>
       </c>
@@ -3428,22 +3467,22 @@
         <f aca="false">WEEKNUM(A24,2)</f>
         <v>52</v>
       </c>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="47" t="n">
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="48" t="n">
         <f aca="false">(E24-D24-F24+G24)</f>
         <v>0</v>
       </c>
-      <c r="I24" s="24"/>
+      <c r="I24" s="25"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="42" t="n">
+      <c r="A25" s="43" t="n">
         <f aca="false">A24+1</f>
         <v>43093</v>
       </c>
-      <c r="B25" s="23" t="n">
+      <c r="B25" s="24" t="n">
         <f aca="false">A25</f>
         <v>43093</v>
       </c>
@@ -3451,22 +3490,22 @@
         <f aca="false">WEEKNUM(A25,2)</f>
         <v>52</v>
       </c>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="47" t="n">
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="48" t="n">
         <f aca="false">(E25-D25-F25+G25)</f>
         <v>0</v>
       </c>
-      <c r="I25" s="43"/>
+      <c r="I25" s="44"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="42" t="n">
+      <c r="A26" s="43" t="n">
         <f aca="false">A25+1</f>
         <v>43094</v>
       </c>
-      <c r="B26" s="23" t="n">
+      <c r="B26" s="24" t="n">
         <f aca="false">A26</f>
         <v>43094</v>
       </c>
@@ -3474,21 +3513,21 @@
         <f aca="false">WEEKNUM(A26,2)</f>
         <v>53</v>
       </c>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="47" t="n">
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="48" t="n">
         <f aca="false">(E26-D26-F26+G26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="42" t="n">
+      <c r="A27" s="43" t="n">
         <f aca="false">A26+1</f>
         <v>43095</v>
       </c>
-      <c r="B27" s="23" t="n">
+      <c r="B27" s="24" t="n">
         <f aca="false">A27</f>
         <v>43095</v>
       </c>
@@ -3496,21 +3535,21 @@
         <f aca="false">WEEKNUM(A27,2)</f>
         <v>53</v>
       </c>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="47" t="n">
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="48" t="n">
         <f aca="false">(E27-D27-F27+G27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="42" t="n">
+      <c r="A28" s="43" t="n">
         <f aca="false">A27+1</f>
         <v>43096</v>
       </c>
-      <c r="B28" s="23" t="n">
+      <c r="B28" s="24" t="n">
         <f aca="false">A28</f>
         <v>43096</v>
       </c>
@@ -3518,21 +3557,21 @@
         <f aca="false">WEEKNUM(A28,2)</f>
         <v>53</v>
       </c>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="47" t="n">
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="48" t="n">
         <f aca="false">(E28-D28-F28+G28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="42" t="n">
+      <c r="A29" s="43" t="n">
         <f aca="false">A28+1</f>
         <v>43097</v>
       </c>
-      <c r="B29" s="23" t="n">
+      <c r="B29" s="24" t="n">
         <f aca="false">A29</f>
         <v>43097</v>
       </c>
@@ -3540,21 +3579,28 @@
         <f aca="false">WEEKNUM(A29,2)</f>
         <v>53</v>
       </c>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="47" t="n">
+      <c r="D29" s="47" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="E29" s="47" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="48" t="n">
         <f aca="false">(E29-D29-F29+G29)</f>
-        <v>0</v>
+        <v>0.0833333333333334</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="42" t="n">
+      <c r="A30" s="43" t="n">
         <f aca="false">A29+1</f>
         <v>43098</v>
       </c>
-      <c r="B30" s="23" t="n">
+      <c r="B30" s="24" t="n">
         <f aca="false">A30</f>
         <v>43098</v>
       </c>
@@ -3562,21 +3608,21 @@
         <f aca="false">WEEKNUM(A30,2)</f>
         <v>53</v>
       </c>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="47" t="n">
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="48" t="n">
         <f aca="false">(E30-D30-F30+G30)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="42" t="n">
+      <c r="A31" s="43" t="n">
         <f aca="false">A30+1</f>
         <v>43099</v>
       </c>
-      <c r="B31" s="23" t="n">
+      <c r="B31" s="24" t="n">
         <f aca="false">A31</f>
         <v>43099</v>
       </c>
@@ -3584,65 +3630,65 @@
         <f aca="false">WEEKNUM(A31,2)</f>
         <v>53</v>
       </c>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="47" t="n">
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="48" t="n">
         <f aca="false">(E31-D31-F31+G31)</f>
         <v>0</v>
       </c>
-      <c r="I31" s="24"/>
+      <c r="I31" s="25"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="48" t="n">
+      <c r="A32" s="49" t="n">
         <f aca="false">A31+1</f>
         <v>43100</v>
       </c>
-      <c r="B32" s="32" t="n">
+      <c r="B32" s="33" t="n">
         <f aca="false">A32</f>
         <v>43100</v>
       </c>
-      <c r="C32" s="33" t="n">
+      <c r="C32" s="34" t="n">
         <f aca="false">WEEKNUM(A32,2)</f>
         <v>53</v>
       </c>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="47" t="n">
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="48" t="n">
         <f aca="false">(E32-D32-F32+G32)</f>
         <v>0</v>
       </c>
-      <c r="I32" s="35"/>
+      <c r="I32" s="36"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="36"/>
+      <c r="A33" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="37"/>
       <c r="C33" s="9" t="n">
         <f aca="false">Zusammenfassung!C9</f>
         <v>1.5</v>
       </c>
-      <c r="H33" s="50"/>
+      <c r="H33" s="51"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="40" t="n">
+      <c r="A34" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="39"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="41" t="n">
         <f aca="false">SUM(H2:H32)</f>
-        <v>2.75416666666667</v>
-      </c>
-      <c r="I34" s="41"/>
+        <v>2.8375</v>
+      </c>
+      <c r="I34" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3720,57 +3766,58 @@
   </sheetPr>
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.4"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="42" t="n">
+      <c r="A2" s="43" t="n">
         <f aca="false">DATE(2018,1,1)</f>
         <v>43101</v>
       </c>
-      <c r="B2" s="23" t="n">
+      <c r="B2" s="24" t="n">
         <f aca="false">A2</f>
         <v>43101</v>
       </c>
@@ -3778,21 +3825,21 @@
         <f aca="false">WEEKNUM(A2,2)</f>
         <v>1</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47" t="n">
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48" t="n">
         <f aca="false">E2-D2-F2+G2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42" t="n">
+      <c r="A3" s="43" t="n">
         <f aca="false">A2+1</f>
         <v>43102</v>
       </c>
-      <c r="B3" s="23" t="n">
+      <c r="B3" s="24" t="n">
         <f aca="false">A3</f>
         <v>43102</v>
       </c>
@@ -3800,21 +3847,21 @@
         <f aca="false">WEEKNUM(A3,2)</f>
         <v>1</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47" t="n">
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48" t="n">
         <f aca="false">E3-D3-F3+G3</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="42" t="n">
+      <c r="A4" s="43" t="n">
         <f aca="false">A3+1</f>
         <v>43103</v>
       </c>
-      <c r="B4" s="23" t="n">
+      <c r="B4" s="24" t="n">
         <f aca="false">A4</f>
         <v>43103</v>
       </c>
@@ -3822,21 +3869,21 @@
         <f aca="false">WEEKNUM(A4,2)</f>
         <v>1</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47" t="n">
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48" t="n">
         <f aca="false">E4-D4-F4+G4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="42" t="n">
+      <c r="A5" s="43" t="n">
         <f aca="false">A4+1</f>
         <v>43104</v>
       </c>
-      <c r="B5" s="23" t="n">
+      <c r="B5" s="24" t="n">
         <f aca="false">A5</f>
         <v>43104</v>
       </c>
@@ -3844,21 +3891,21 @@
         <f aca="false">WEEKNUM(A5,2)</f>
         <v>1</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47" t="n">
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48" t="n">
         <f aca="false">E5-D5-F5+G5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="42" t="n">
+      <c r="A6" s="43" t="n">
         <f aca="false">A5+1</f>
         <v>43105</v>
       </c>
-      <c r="B6" s="23" t="n">
+      <c r="B6" s="24" t="n">
         <f aca="false">A6</f>
         <v>43105</v>
       </c>
@@ -3866,21 +3913,21 @@
         <f aca="false">WEEKNUM(A6,2)</f>
         <v>1</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47" t="n">
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48" t="n">
         <f aca="false">E6-D6-F6+G6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="42" t="n">
+      <c r="A7" s="43" t="n">
         <f aca="false">A6+1</f>
         <v>43106</v>
       </c>
-      <c r="B7" s="23" t="n">
+      <c r="B7" s="24" t="n">
         <f aca="false">A7</f>
         <v>43106</v>
       </c>
@@ -3888,22 +3935,22 @@
         <f aca="false">WEEKNUM(A7,2)</f>
         <v>1</v>
       </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47" t="n">
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48" t="n">
         <f aca="false">E7-D7-F7+G7</f>
         <v>0</v>
       </c>
-      <c r="I7" s="24"/>
+      <c r="I7" s="25"/>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="42" t="n">
+      <c r="A8" s="43" t="n">
         <f aca="false">A7+1</f>
         <v>43107</v>
       </c>
-      <c r="B8" s="23" t="n">
+      <c r="B8" s="24" t="n">
         <f aca="false">A8</f>
         <v>43107</v>
       </c>
@@ -3911,28 +3958,28 @@
         <f aca="false">WEEKNUM(A8,2)</f>
         <v>1</v>
       </c>
-      <c r="D8" s="47" t="n">
+      <c r="D8" s="48" t="n">
         <v>0.625</v>
       </c>
-      <c r="E8" s="47" t="n">
+      <c r="E8" s="48" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47" t="n">
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48" t="n">
         <f aca="false">E8-D8-F8+G8</f>
         <v>0.0833333333333334</v>
       </c>
-      <c r="I8" s="43" t="s">
-        <v>55</v>
+      <c r="I8" s="44" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="42" t="n">
+      <c r="A9" s="43" t="n">
         <f aca="false">A8+1</f>
         <v>43108</v>
       </c>
-      <c r="B9" s="23" t="n">
+      <c r="B9" s="24" t="n">
         <f aca="false">A9</f>
         <v>43108</v>
       </c>
@@ -3940,21 +3987,21 @@
         <f aca="false">WEEKNUM(A9,2)</f>
         <v>2</v>
       </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47" t="n">
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48" t="n">
         <f aca="false">E9-D9-F9+G9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="42" t="n">
+      <c r="A10" s="43" t="n">
         <f aca="false">A9+1</f>
         <v>43109</v>
       </c>
-      <c r="B10" s="23" t="n">
+      <c r="B10" s="24" t="n">
         <f aca="false">A10</f>
         <v>43109</v>
       </c>
@@ -3962,21 +4009,28 @@
         <f aca="false">WEEKNUM(A10,2)</f>
         <v>2</v>
       </c>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47" t="n">
+      <c r="D10" s="48" t="n">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="E10" s="48" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48" t="n">
         <f aca="false">E10-D10-F10+G10</f>
-        <v>0</v>
+        <v>0.0416666666666666</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="42" t="n">
+      <c r="A11" s="43" t="n">
         <f aca="false">A10+1</f>
         <v>43110</v>
       </c>
-      <c r="B11" s="23" t="n">
+      <c r="B11" s="24" t="n">
         <f aca="false">A11</f>
         <v>43110</v>
       </c>
@@ -3984,30 +4038,30 @@
         <f aca="false">WEEKNUM(A11,2)</f>
         <v>2</v>
       </c>
-      <c r="D11" s="47" t="n">
+      <c r="D11" s="48" t="n">
         <v>0.34375</v>
       </c>
-      <c r="E11" s="47" t="n">
+      <c r="E11" s="48" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="F11" s="47" t="n">
+      <c r="F11" s="48" t="n">
         <v>0.0833333333333333</v>
       </c>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47" t="n">
+      <c r="G11" s="48"/>
+      <c r="H11" s="48" t="n">
         <f aca="false">E11-D11-F11+G11</f>
         <v>0.28125</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="42" t="n">
+      <c r="A12" s="43" t="n">
         <f aca="false">A11+1</f>
         <v>43111</v>
       </c>
-      <c r="B12" s="23" t="n">
+      <c r="B12" s="24" t="n">
         <f aca="false">A12</f>
         <v>43111</v>
       </c>
@@ -4015,30 +4069,30 @@
         <f aca="false">WEEKNUM(A12,2)</f>
         <v>2</v>
       </c>
-      <c r="D12" s="47" t="n">
+      <c r="D12" s="48" t="n">
         <v>0.510416666666667</v>
       </c>
-      <c r="E12" s="47" t="n">
+      <c r="E12" s="48" t="n">
         <v>0.675</v>
       </c>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47" t="n">
+      <c r="F12" s="48"/>
+      <c r="G12" s="48" t="n">
         <v>0.03125</v>
       </c>
-      <c r="H12" s="47" t="n">
+      <c r="H12" s="48" t="n">
         <f aca="false">E12-D12-F12+G12</f>
         <v>0.195833333333333</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="44" t="n">
+      <c r="A13" s="45" t="n">
         <f aca="false">A12+1</f>
         <v>43112</v>
       </c>
-      <c r="B13" s="26" t="n">
+      <c r="B13" s="27" t="n">
         <f aca="false">A13</f>
         <v>43112</v>
       </c>
@@ -4046,29 +4100,29 @@
         <f aca="false">WEEKNUM(A13,2)</f>
         <v>2</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47" t="n">
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48" t="n">
         <v>0.138888888888889</v>
       </c>
-      <c r="H13" s="47" t="n">
+      <c r="H13" s="48" t="n">
         <f aca="false">E13-D13-F13+G13</f>
         <v>0.138888888888889</v>
       </c>
-      <c r="I13" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
+      <c r="I13" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
     </row>
     <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="42" t="n">
+      <c r="A14" s="43" t="n">
         <f aca="false">A13+1</f>
         <v>43113</v>
       </c>
-      <c r="B14" s="23" t="n">
+      <c r="B14" s="24" t="n">
         <f aca="false">A14</f>
         <v>43113</v>
       </c>
@@ -4076,33 +4130,33 @@
         <f aca="false">WEEKNUM(A14,2)</f>
         <v>2</v>
       </c>
-      <c r="D14" s="47" t="n">
+      <c r="D14" s="48" t="n">
         <v>0.5625</v>
       </c>
-      <c r="E14" s="47" t="n">
+      <c r="E14" s="48" t="n">
         <v>0.875</v>
       </c>
-      <c r="F14" s="47" t="n">
+      <c r="F14" s="48" t="n">
         <v>0.0625</v>
       </c>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47" t="n">
+      <c r="G14" s="48"/>
+      <c r="H14" s="48" t="n">
         <f aca="false">E14-D14-F14+G14</f>
         <v>0.25</v>
       </c>
-      <c r="I14" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="52"/>
+      <c r="I14" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="53"/>
     </row>
     <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="42" t="n">
+      <c r="A15" s="43" t="n">
         <f aca="false">A14+1</f>
         <v>43114</v>
       </c>
-      <c r="B15" s="23" t="n">
+      <c r="B15" s="24" t="n">
         <f aca="false">A15</f>
         <v>43114</v>
       </c>
@@ -4110,33 +4164,33 @@
         <f aca="false">WEEKNUM(A15,2)</f>
         <v>2</v>
       </c>
-      <c r="D15" s="47" t="n">
+      <c r="D15" s="48" t="n">
         <v>0.5625</v>
       </c>
-      <c r="E15" s="47" t="n">
+      <c r="E15" s="48" t="n">
         <v>1.0375</v>
       </c>
-      <c r="F15" s="47" t="n">
+      <c r="F15" s="48" t="n">
         <v>0.1875</v>
       </c>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47" t="n">
+      <c r="G15" s="48"/>
+      <c r="H15" s="48" t="n">
         <f aca="false">E15-D15-F15+G15</f>
         <v>0.2875</v>
       </c>
-      <c r="I15" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="52"/>
+      <c r="I15" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="53"/>
     </row>
     <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="42" t="n">
+      <c r="A16" s="43" t="n">
         <f aca="false">A15+1</f>
         <v>43115</v>
       </c>
-      <c r="B16" s="23" t="n">
+      <c r="B16" s="24" t="n">
         <f aca="false">A16</f>
         <v>43115</v>
       </c>
@@ -4144,27 +4198,33 @@
         <f aca="false">WEEKNUM(A16,2)</f>
         <v>3</v>
       </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47" t="n">
+      <c r="D16" s="48" t="n">
+        <v>0.604166666666667</v>
+      </c>
+      <c r="E16" s="48" t="n">
+        <v>0.729166666666667</v>
+      </c>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48" t="n">
+        <v>0.0208333333333333</v>
+      </c>
+      <c r="H16" s="48" t="n">
         <f aca="false">E16-D16-F16+G16</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="52"/>
+        <v>0.145833333333333</v>
+      </c>
+      <c r="I16" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="53"/>
     </row>
     <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="42" t="n">
+      <c r="A17" s="43" t="n">
         <f aca="false">A16+1</f>
         <v>43116</v>
       </c>
-      <c r="B17" s="23" t="n">
+      <c r="B17" s="24" t="n">
         <f aca="false">A17</f>
         <v>43116</v>
       </c>
@@ -4172,25 +4232,25 @@
         <f aca="false">WEEKNUM(A17,2)</f>
         <v>3</v>
       </c>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47" t="n">
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48" t="n">
         <f aca="false">E17-D17-F17+G17</f>
         <v>0</v>
       </c>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="53"/>
     </row>
     <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="42" t="n">
+      <c r="A18" s="43" t="n">
         <f aca="false">A17+1</f>
         <v>43117</v>
       </c>
-      <c r="B18" s="23" t="n">
+      <c r="B18" s="24" t="n">
         <f aca="false">A18</f>
         <v>43117</v>
       </c>
@@ -4198,25 +4258,25 @@
         <f aca="false">WEEKNUM(A18,2)</f>
         <v>3</v>
       </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47" t="n">
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48" t="n">
         <f aca="false">E18-D18-F18+G18</f>
         <v>0</v>
       </c>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="53"/>
     </row>
     <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="42" t="n">
+      <c r="A19" s="43" t="n">
         <f aca="false">A18+1</f>
         <v>43118</v>
       </c>
-      <c r="B19" s="23" t="n">
+      <c r="B19" s="24" t="n">
         <f aca="false">A19</f>
         <v>43118</v>
       </c>
@@ -4224,25 +4284,29 @@
         <f aca="false">WEEKNUM(A19,2)</f>
         <v>3</v>
       </c>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47" t="n">
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="H19" s="48" t="n">
         <f aca="false">E19-D19-F19+G19</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="52"/>
+        <v>0.0625</v>
+      </c>
+      <c r="I19" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="53"/>
     </row>
     <row r="20" s="1" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="44" t="n">
+      <c r="A20" s="45" t="n">
         <f aca="false">A19+1</f>
         <v>43119</v>
       </c>
-      <c r="B20" s="26" t="n">
+      <c r="B20" s="27" t="n">
         <f aca="false">A20</f>
         <v>43119</v>
       </c>
@@ -4250,27 +4314,29 @@
         <f aca="false">WEEKNUM(A20,2)</f>
         <v>3</v>
       </c>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47" t="n">
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="H20" s="48" t="n">
         <f aca="false">E20-D20-F20+G20</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
+        <v>0.0625</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
     </row>
     <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="42" t="n">
+      <c r="A21" s="43" t="n">
         <f aca="false">A20+1</f>
         <v>43120</v>
       </c>
-      <c r="B21" s="23" t="n">
+      <c r="B21" s="24" t="n">
         <f aca="false">A21</f>
         <v>43120</v>
       </c>
@@ -4278,22 +4344,30 @@
         <f aca="false">WEEKNUM(A21,2)</f>
         <v>3</v>
       </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47" t="n">
+      <c r="D21" s="48" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="E21" s="48" t="n">
+        <v>0.833333333333333</v>
+      </c>
+      <c r="F21" s="48" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48" t="n">
         <f aca="false">E21-D21-F21+G21</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="24"/>
+        <v>0.220833333333333</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="42" t="n">
+      <c r="A22" s="43" t="n">
         <f aca="false">A21+1</f>
         <v>43121</v>
       </c>
-      <c r="B22" s="23" t="n">
+      <c r="B22" s="24" t="n">
         <f aca="false">A22</f>
         <v>43121</v>
       </c>
@@ -4301,22 +4375,22 @@
         <f aca="false">WEEKNUM(A22,2)</f>
         <v>3</v>
       </c>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47" t="n">
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48" t="n">
         <f aca="false">E22-D22-F22+G22</f>
         <v>0</v>
       </c>
-      <c r="I22" s="24"/>
+      <c r="I22" s="25"/>
     </row>
     <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="42" t="n">
+      <c r="A23" s="43" t="n">
         <f aca="false">A22+1</f>
         <v>43122</v>
       </c>
-      <c r="B23" s="23" t="n">
+      <c r="B23" s="24" t="n">
         <f aca="false">A23</f>
         <v>43122</v>
       </c>
@@ -4324,21 +4398,21 @@
         <f aca="false">WEEKNUM(A23,2)</f>
         <v>4</v>
       </c>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47" t="n">
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48" t="n">
         <f aca="false">E23-D23-F23+G23</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="42" t="n">
+      <c r="A24" s="43" t="n">
         <f aca="false">A23+1</f>
         <v>43123</v>
       </c>
-      <c r="B24" s="23" t="n">
+      <c r="B24" s="24" t="n">
         <f aca="false">A24</f>
         <v>43123</v>
       </c>
@@ -4346,21 +4420,21 @@
         <f aca="false">WEEKNUM(A24,2)</f>
         <v>4</v>
       </c>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47" t="n">
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48" t="n">
         <f aca="false">E24-D24-F24+G24</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="42" t="n">
+      <c r="A25" s="43" t="n">
         <f aca="false">A24+1</f>
         <v>43124</v>
       </c>
-      <c r="B25" s="23" t="n">
+      <c r="B25" s="24" t="n">
         <f aca="false">A25</f>
         <v>43124</v>
       </c>
@@ -4368,21 +4442,21 @@
         <f aca="false">WEEKNUM(A25,2)</f>
         <v>4</v>
       </c>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47" t="n">
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48" t="n">
         <f aca="false">E25-D25-F25+G25</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="42" t="n">
+      <c r="A26" s="43" t="n">
         <f aca="false">A25+1</f>
         <v>43125</v>
       </c>
-      <c r="B26" s="23" t="n">
+      <c r="B26" s="24" t="n">
         <f aca="false">A26</f>
         <v>43125</v>
       </c>
@@ -4390,21 +4464,21 @@
         <f aca="false">WEEKNUM(A26,2)</f>
         <v>4</v>
       </c>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47" t="n">
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48" t="n">
         <f aca="false">E26-D26-F26+G26</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="42" t="n">
+      <c r="A27" s="43" t="n">
         <f aca="false">A26+1</f>
         <v>43126</v>
       </c>
-      <c r="B27" s="23" t="n">
+      <c r="B27" s="24" t="n">
         <f aca="false">A27</f>
         <v>43126</v>
       </c>
@@ -4412,21 +4486,21 @@
         <f aca="false">WEEKNUM(A27,2)</f>
         <v>4</v>
       </c>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47" t="n">
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48" t="n">
         <f aca="false">E27-D27-F27+G27</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="42" t="n">
+      <c r="A28" s="43" t="n">
         <f aca="false">A27+1</f>
         <v>43127</v>
       </c>
-      <c r="B28" s="23" t="n">
+      <c r="B28" s="24" t="n">
         <f aca="false">A28</f>
         <v>43127</v>
       </c>
@@ -4434,22 +4508,22 @@
         <f aca="false">WEEKNUM(A28,2)</f>
         <v>4</v>
       </c>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47" t="n">
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48" t="n">
         <f aca="false">E28-D28-F28+G28</f>
         <v>0</v>
       </c>
-      <c r="I28" s="24"/>
+      <c r="I28" s="25"/>
     </row>
     <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="42" t="n">
+      <c r="A29" s="43" t="n">
         <f aca="false">A28+1</f>
         <v>43128</v>
       </c>
-      <c r="B29" s="23" t="n">
+      <c r="B29" s="24" t="n">
         <f aca="false">A29</f>
         <v>43128</v>
       </c>
@@ -4457,22 +4531,22 @@
         <f aca="false">WEEKNUM(A29,2)</f>
         <v>4</v>
       </c>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47" t="n">
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48" t="n">
         <f aca="false">E29-D29-F29+G29</f>
         <v>0</v>
       </c>
-      <c r="I29" s="43"/>
+      <c r="I29" s="44"/>
     </row>
     <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="42" t="n">
+      <c r="A30" s="43" t="n">
         <f aca="false">A29+1</f>
         <v>43129</v>
       </c>
-      <c r="B30" s="23" t="n">
+      <c r="B30" s="24" t="n">
         <f aca="false">A30</f>
         <v>43129</v>
       </c>
@@ -4480,21 +4554,21 @@
         <f aca="false">WEEKNUM(A30,2)</f>
         <v>5</v>
       </c>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47" t="n">
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48" t="n">
         <f aca="false">E30-D30-F30+G30</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="42" t="n">
+      <c r="A31" s="43" t="n">
         <f aca="false">A30+1</f>
         <v>43130</v>
       </c>
-      <c r="B31" s="23" t="n">
+      <c r="B31" s="24" t="n">
         <f aca="false">A31</f>
         <v>43130</v>
       </c>
@@ -4502,64 +4576,64 @@
         <f aca="false">WEEKNUM(A31,2)</f>
         <v>5</v>
       </c>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47" t="n">
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48" t="n">
         <f aca="false">E31-D31-F31+G31</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="48" t="n">
+      <c r="A32" s="49" t="n">
         <f aca="false">A31+1</f>
         <v>43131</v>
       </c>
-      <c r="B32" s="32" t="n">
+      <c r="B32" s="33" t="n">
         <f aca="false">A32</f>
         <v>43131</v>
       </c>
-      <c r="C32" s="33" t="n">
+      <c r="C32" s="34" t="n">
         <f aca="false">WEEKNUM(A32,2)</f>
         <v>5</v>
       </c>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="47" t="n">
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="48" t="n">
         <f aca="false">E32-D32-F32+G32</f>
         <v>0</v>
       </c>
-      <c r="I32" s="35"/>
+      <c r="I32" s="36"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="36"/>
+      <c r="A33" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="37"/>
       <c r="C33" s="9" t="n">
         <f aca="false">Zusammenfassung!C10</f>
         <v>1.875</v>
       </c>
-      <c r="H33" s="54"/>
+      <c r="H33" s="55"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="40" t="n">
+      <c r="A34" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="39"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="41" t="n">
         <f aca="false">SUM(H2:H32)</f>
-        <v>1.23680555555556</v>
-      </c>
-      <c r="I34" s="41"/>
+        <v>1.77013888888889</v>
+      </c>
+      <c r="I34" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>